<commit_message>
Update add-in custom functions and tidy up example files
</commit_message>
<xml_diff>
--- a/export/examples/test.xlsx
+++ b/export/examples/test.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abhis\Documents\Github Projects\Server\excel-stream-add-in\stream-add-in\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abhis\Documents\Github Projects\Server\excel-stream\example-excel-addin\export\examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D9122BC-630F-46DE-9E62-16AF26E24858}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25EDCD99-B8A5-4103-AE2E-79106F0134F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2295" yWindow="1935" windowWidth="25275" windowHeight="13440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15675" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -559,10 +559,14 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="11" fillId="6" borderId="4" xfId="11" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="13" fillId="7" borderId="7" xfId="13" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="13" fillId="7" borderId="7" xfId="13" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" xfId="11"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -918,7 +922,7 @@
 
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
-  <wetp:taskpane dockstate="" visibility="1" width="700" row="2">
+  <wetp:taskpane dockstate="" visibility="1" width="700" row="3">
     <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </wetp:taskpane>
 </wetp:taskpanes>
@@ -954,141 +958,169 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C3:K13"/>
+  <dimension ref="A1:K18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
+    <col min="1" max="2" width="16.265625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.06640625" customWidth="1"/>
-    <col min="5" max="5" width="8.3984375" customWidth="1"/>
-    <col min="6" max="6" width="7.59765625" customWidth="1"/>
-    <col min="7" max="7" width="5.19921875" customWidth="1"/>
+    <col min="4" max="4" width="16.265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.1328125" customWidth="1"/>
+    <col min="6" max="6" width="10.265625" customWidth="1"/>
+    <col min="7" max="7" width="9.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:11" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A1" s="5"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
       <c r="E3" cm="1">
-        <f t="array" ref="E3:F5">TRANSPOSE(_xldudf_STREAM_SUBSCRIBE("random.matrix", ""))</f>
-        <v>-59</v>
+        <f t="array" ref="E3:F5">TRANSPOSE(_xldudf_STREAM_SUBSCRIBE("random.matrix", "data"))</f>
+        <v>14</v>
       </c>
       <c r="F3">
-        <v>7</v>
-      </c>
-      <c r="G3">
+        <v>25</v>
+      </c>
+      <c r="G3" s="6">
         <f>SUM(E3:F3)</f>
-        <v>-52</v>
+        <v>39</v>
       </c>
       <c r="J3" cm="1">
-        <f t="array" ref="J3:K5">TRANSPOSE(_xldudf_STREAM_SUBSCRIBE("random.matrix", ""))</f>
-        <v>-59</v>
+        <f t="array" ref="J3:K5">TRANSPOSE(_xldudf_STREAM_SUBSCRIBE("random.matrix", "data"))</f>
+        <v>14</v>
       </c>
       <c r="K3">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="3:11" x14ac:dyDescent="0.45">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
       <c r="E4">
-        <v>41</v>
+        <v>-27</v>
       </c>
       <c r="F4">
-        <v>-12</v>
-      </c>
-      <c r="G4">
+        <v>-47</v>
+      </c>
+      <c r="G4" s="6">
         <f t="shared" ref="G4:G5" si="0">SUM(E4:F4)</f>
-        <v>29</v>
+        <v>-74</v>
       </c>
       <c r="J4">
-        <v>41</v>
+        <v>-27</v>
       </c>
       <c r="K4">
-        <v>-12</v>
-      </c>
-    </row>
-    <row r="5" spans="3:11" x14ac:dyDescent="0.45">
+        <v>-47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="E5">
-        <v>-53</v>
+        <v>60</v>
       </c>
       <c r="F5">
-        <v>39</v>
-      </c>
-      <c r="G5">
+        <v>-10</v>
+      </c>
+      <c r="G5" s="6">
         <f t="shared" si="0"/>
-        <v>-14</v>
+        <v>50</v>
       </c>
       <c r="J5">
-        <v>-53</v>
+        <v>60</v>
       </c>
       <c r="K5">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="6" spans="3:11" x14ac:dyDescent="0.45">
-      <c r="C6" s="1" cm="1">
-        <f t="array" ref="C6">_xldudf_STREAM_SUBSCRIBE("test.time", "")</f>
-        <v>1692745489047</v>
-      </c>
-      <c r="E6">
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="C6" s="3" cm="1">
+        <f t="array" ref="C6">_xldudf_STREAM_SUBSCRIBE("test.time", "data")</f>
+        <v>1693774704627</v>
+      </c>
+      <c r="E6" s="6">
         <f>SUM(E3:E5)</f>
-        <v>-71</v>
-      </c>
-      <c r="F6">
+        <v>47</v>
+      </c>
+      <c r="F6" s="6">
         <f>SUM(F3:F5)</f>
-        <v>34</v>
-      </c>
-    </row>
-    <row r="7" spans="3:11" x14ac:dyDescent="0.45">
+        <v>-32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
       <c r="J7" cm="1">
         <f t="array" ref="J7:K9">E3:F5</f>
-        <v>-59</v>
+        <v>14</v>
       </c>
       <c r="K7">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="3:11" x14ac:dyDescent="0.45">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="J8">
-        <v>41</v>
+        <v>-27</v>
       </c>
       <c r="K8">
-        <v>-12</v>
-      </c>
-    </row>
-    <row r="9" spans="3:11" x14ac:dyDescent="0.45">
-      <c r="C9" s="2" cm="1">
-        <f t="array" ref="C9:C13">TRANSPOSE(_xldudf_STREAM_HISTORY("C6", 5))</f>
-        <v>1692745487850</v>
-      </c>
-      <c r="E9" s="1">
+        <v>-47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="C9" s="4" cm="1">
+        <f t="array" ref="C9:C13">TRANSPOSE(_xldudf_STREAM_HISTORY("C6",5))</f>
+        <v>1693774703311</v>
+      </c>
+      <c r="E9" s="2">
         <f>C13-C9</f>
-        <v>978</v>
+        <v>1097</v>
       </c>
       <c r="J9">
-        <v>-53</v>
+        <v>60</v>
       </c>
       <c r="K9">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="10" spans="3:11" x14ac:dyDescent="0.45">
-      <c r="C10" s="2">
-        <v>1692745488068</v>
-      </c>
-    </row>
-    <row r="11" spans="3:11" x14ac:dyDescent="0.45">
-      <c r="C11" s="2">
-        <v>1692745488281</v>
-      </c>
-    </row>
-    <row r="12" spans="3:11" x14ac:dyDescent="0.45">
-      <c r="C12" s="2">
-        <v>1692745488609</v>
-      </c>
-    </row>
-    <row r="13" spans="3:11" x14ac:dyDescent="0.45">
-      <c r="C13" s="2">
-        <v>1692745488828</v>
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="C10" s="4">
+        <v>1693774703639</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="C11" s="4">
+        <v>1693774703858</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="C12" s="4">
+        <v>1693774704189</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="C13" s="4">
+        <v>1693774704408</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="14.65" thickTop="1" x14ac:dyDescent="0.45"/>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A18" s="1" cm="1">
+        <f t="array" ref="A18:E18">_xldudf_STREAM_HISTORY("C6",5)</f>
+        <v>1693774703311</v>
+      </c>
+      <c r="B18" s="1">
+        <v>1693774703639</v>
+      </c>
+      <c r="C18" s="1">
+        <v>1693774703858</v>
+      </c>
+      <c r="D18" s="1">
+        <v>1693774704189</v>
+      </c>
+      <c r="E18" s="1">
+        <v>1693774704408</v>
       </c>
     </row>
   </sheetData>

</xml_diff>